<commit_message>
updated phase 1 grading, error file included
</commit_message>
<xml_diff>
--- a/project1-grading.xlsx
+++ b/project1-grading.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Area</t>
   </si>
@@ -100,14 +100,53 @@
     <t>Programs need to be commented.</t>
   </si>
   <si>
-    <t>Though your programs look very good, you didn't have any instructions how to run the program. I can't reproduce the results you claimed. When compiling the programs using the "Makefile" multiple errors occurred. This could be the results that you are in the middle of working on phase two of the program?</t>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> 28</t>
+    </r>
+  </si>
+  <si>
+    <t>Though your programs look very good, you didn't have any instructions how to run the program. I can't reproduce the results you claimed. When compiling the programs using the "Makefile" multiple errors occurred. This could be the results that you are in the middle of working on phase two of the program?
+Thank you for the updated instructions. The "make" errors are probably due to the fact that you are working on Phase 2 of the program.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> 25</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -165,6 +204,13 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -539,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -706,6 +752,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,8 +1130,8 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1137,7 +1186,7 @@
       <c r="D5" s="16"/>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="1:5" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="267.75" x14ac:dyDescent="0.2">
       <c r="A6" s="61"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -1145,11 +1194,11 @@
       <c r="C6" s="10">
         <v>30</v>
       </c>
-      <c r="D6" s="7">
-        <v>22</v>
+      <c r="D6" s="63" t="s">
+        <v>27</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1167,8 +1216,8 @@
       <c r="C8" s="10">
         <v>25</v>
       </c>
-      <c r="D8" s="7">
-        <v>18</v>
+      <c r="D8" s="63" t="s">
+        <v>29</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>24</v>
@@ -1291,8 +1340,7 @@
         <v>100</v>
       </c>
       <c r="D20" s="32">
-        <f>SUM(D6:D19)</f>
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E20" s="19"/>
     </row>

</xml_diff>

<commit_message>
Updating project1 grading comments
</commit_message>
<xml_diff>
--- a/project1-grading.xlsx
+++ b/project1-grading.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>Area</t>
   </si>
@@ -140,6 +140,27 @@
       </rPr>
       <t xml:space="preserve"> 25</t>
     </r>
+  </si>
+  <si>
+    <t>Very good! I wish you could combine the two files, handin-phase2.txt and READ.me so it is easier to read. Maybe duplicate the information in READ.me into handin-phase2.txt. Just a thought.</t>
+  </si>
+  <si>
+    <t>It looks fine. But since I was able to use only the query word "bucknell" to find a return link, I don't have a feel how the page would look like if you have multiple return pages.</t>
+  </si>
+  <si>
+    <t>Very good.</t>
+  </si>
+  <si>
+    <t>Excellent.</t>
+  </si>
+  <si>
+    <t>You need to provide more comprehensive comments to your programs.</t>
+  </si>
+  <si>
+    <t>Very good!</t>
+  </si>
+  <si>
+    <t>The server seems to be working fine. It isn't clear, however, that what are the pages collected. When I tested the program, I had no clue what words I should use in query. Most of the words I typed such as "comptuer", "network", "course" end up with no results. Why the home page is titled "Web Crawler"? It doesn't seem to make sense. Come up a better name.</t>
   </si>
 </sst>
 </file>
@@ -747,14 +768,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1130,8 +1151,8 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1199,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1187,14 +1208,14 @@
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" ht="267.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="10">
         <v>30</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="61" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="19" t="s">
@@ -1202,21 +1223,21 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="61"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="5"/>
       <c r="C7" s="12"/>
       <c r="D7" s="9"/>
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="61"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="10">
         <v>25</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="61" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="19" t="s">
@@ -1224,14 +1245,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="61"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="44"/>
       <c r="C9" s="11"/>
       <c r="D9" s="8"/>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="29" t="s">
         <v>20</v>
       </c>
@@ -1246,20 +1267,20 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="5"/>
       <c r="C11" s="12"/>
       <c r="D11" s="9"/>
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="62"/>
       <c r="C12" s="11"/>
       <c r="D12" s="33"/>
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1268,7 +1289,7 @@
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="61"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
@@ -1283,14 +1304,14 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="61"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="58"/>
       <c r="C15" s="59"/>
       <c r="D15" s="60"/>
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="29" t="s">
         <v>10</v>
       </c>
@@ -1345,17 +1366,17 @@
       <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="62"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="30"/>
       <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="25"/>
       <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="62"/>
+      <c r="A23" s="63"/>
       <c r="B23" s="43" t="s">
         <v>14</v>
       </c>
@@ -1384,47 +1405,59 @@
       <c r="D25" s="16"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="216.75" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="10">
         <v>20</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="7">
+        <v>18</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="12"/>
       <c r="D27" s="9"/>
       <c r="E27" s="19"/>
     </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B28" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="11">
         <v>10</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D28" s="8">
+        <v>9</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="44"/>
       <c r="C29" s="11"/>
       <c r="D29" s="8"/>
       <c r="E29" s="19"/>
     </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="10">
         <v>15</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="19"/>
+      <c r="D30" s="7">
+        <v>14</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
@@ -1439,8 +1472,12 @@
       <c r="C32" s="24">
         <v>15</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="19"/>
+      <c r="D32" s="42">
+        <v>15</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="33" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="20"/>
@@ -1468,8 +1505,12 @@
       <c r="C36" s="10">
         <v>15</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="19"/>
+      <c r="D36" s="7">
+        <v>15</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="29"/>
@@ -1477,15 +1518,19 @@
       <c r="D37" s="8"/>
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C38" s="11">
         <v>15</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="19"/>
+      <c r="D38" s="8">
+        <v>13</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="39" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="36"/>
@@ -1500,8 +1545,12 @@
       <c r="C40" s="40">
         <v>10</v>
       </c>
-      <c r="D40" s="35"/>
-      <c r="E40" s="19"/>
+      <c r="D40" s="35">
+        <v>7</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="41" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="29"/>
@@ -1518,7 +1567,7 @@
       </c>
       <c r="D42" s="32">
         <f>SUM(D26:D41)</f>
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated project 1 part 2 grade
</commit_message>
<xml_diff>
--- a/project1-grading.xlsx
+++ b/project1-grading.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>Area</t>
   </si>
@@ -162,12 +162,48 @@
   <si>
     <t>The server seems to be working fine. It isn't clear, however, that what are the pages collected. When I tested the program, I had no clue what words I should use in query. Most of the words I typed such as "comptuer", "network", "course" end up with no results. Why the home page is titled "Web Crawler"? It doesn't seem to make sense. Come up a better name.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> 19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t xml:space="preserve"> 15</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -229,6 +265,12 @@
       <strike/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -1151,8 +1193,8 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1412,8 +1454,8 @@
       <c r="C26" s="10">
         <v>20</v>
       </c>
-      <c r="D26" s="7">
-        <v>18</v>
+      <c r="D26" s="61" t="s">
+        <v>37</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>36</v>
@@ -1452,8 +1494,8 @@
       <c r="C30" s="10">
         <v>15</v>
       </c>
-      <c r="D30" s="7">
-        <v>14</v>
+      <c r="D30" s="61" t="s">
+        <v>38</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>31</v>
@@ -1566,8 +1608,7 @@
         <v>100</v>
       </c>
       <c r="D42" s="32">
-        <f>SUM(D26:D41)</f>
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15" x14ac:dyDescent="0.2">

</xml_diff>